<commit_message>
change excel file and fixed bugs
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/LyricsData.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/LyricsData.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\rap.zap.snap\RapZapSnap\Assets\Chew\script\Excel Related\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16530" yWindow="-195" windowWidth="6315" windowHeight="9840" tabRatio="611" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="12120" yWindow="0" windowWidth="16680" windowHeight="12645" tabRatio="611" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="tokiwa1" sheetId="1" r:id="rId1"/>
@@ -22,12 +17,24 @@
     <sheet name="mari2" sheetId="8" r:id="rId8"/>
     <sheet name="mari3" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>delaytime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wholedelay</t>
+    <phoneticPr fontId="1"/>
+  </si>
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -44,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -90,7 +97,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -106,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -148,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,7 +190,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C92" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -405,13 +412,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -492,8 +499,8 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>0.5/9</f>
-        <v>5.5555555555555552E-2</v>
+        <f>0.4/9</f>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -501,8 +508,8 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B18" si="0">0.5/9</f>
-        <v>5.5555555555555552E-2</v>
+        <f t="shared" ref="B11:B18" si="0">0.4/9</f>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -511,7 +518,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -520,7 +527,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -529,7 +536,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -538,7 +545,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -547,7 +554,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
@@ -556,7 +563,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -565,10 +572,10 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="C18">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -576,7 +583,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -584,7 +591,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -592,7 +599,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -600,7 +607,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -608,7 +615,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C23">
         <v>0.1</v>
@@ -649,7 +656,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C27">
         <v>0.1</v>
@@ -660,7 +667,8 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.1</v>
+        <f>0.2/9</f>
+        <v>2.2222222222222223E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -668,7 +676,8 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.1</v>
+        <f t="shared" ref="B29:B35" si="2">0.8/9</f>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
@@ -676,7 +685,8 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -684,7 +694,8 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -692,7 +703,8 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -700,7 +712,8 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -708,7 +721,8 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -716,7 +730,8 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="C35">
         <v>0.2</v>
@@ -766,7 +781,8 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.1</v>
+        <f>0.1/7</f>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -774,7 +790,8 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>0.1</v>
+        <f t="shared" ref="B41:B47" si="3">0.1/7</f>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -782,7 +799,8 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -790,7 +808,8 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -798,7 +817,8 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -806,7 +826,8 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -814,7 +835,8 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>1.4285714285714287E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -822,7 +844,8 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>1.4285714285714287E-2</v>
       </c>
       <c r="C47">
         <v>0.2</v>
@@ -842,7 +865,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <f t="shared" ref="B49:B50" si="2">0.5/3</f>
+        <f t="shared" ref="B49:B50" si="4">0.5/3</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -851,7 +874,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="C50">
@@ -863,7 +886,8 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.04</v>
+        <f>0.3/10</f>
+        <v>0.03</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -871,7 +895,8 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.04</v>
+        <f t="shared" ref="B52:B61" si="5">0.3/10</f>
+        <v>0.03</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -879,7 +904,8 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -887,7 +913,8 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
@@ -895,7 +922,8 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -903,7 +931,8 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
@@ -911,7 +940,8 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -919,7 +949,8 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -927,7 +958,8 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
@@ -935,7 +967,8 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -943,7 +976,8 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0.04</v>
+        <f t="shared" si="5"/>
+        <v>0.03</v>
       </c>
       <c r="C61">
         <v>1.1000000000000001</v>
@@ -954,8 +988,8 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <f>0.4/5</f>
-        <v>0.08</v>
+        <f>0.3/5</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -963,8 +997,8 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <f t="shared" ref="B63:B66" si="3">0.4/5</f>
-        <v>0.08</v>
+        <f t="shared" ref="B63:B66" si="6">0.3/5</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -972,8 +1006,8 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <f t="shared" si="3"/>
-        <v>0.08</v>
+        <f t="shared" si="6"/>
+        <v>0.06</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -981,8 +1015,8 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <f t="shared" si="3"/>
-        <v>0.08</v>
+        <f t="shared" si="6"/>
+        <v>0.06</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -990,8 +1024,8 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f t="shared" si="3"/>
-        <v>0.08</v>
+        <f t="shared" si="6"/>
+        <v>0.06</v>
       </c>
       <c r="C66">
         <v>0.1</v>
@@ -1002,7 +1036,8 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>0.1</v>
+        <f>0.1/9</f>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -1010,7 +1045,8 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0.1</v>
+        <f>0.1/9</f>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -1018,7 +1054,8 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.1</v>
+        <f t="shared" ref="B69:B76" si="7">0.1/9</f>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -1026,7 +1063,8 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -1034,7 +1072,8 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -1042,7 +1081,8 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -1050,7 +1090,8 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -1058,7 +1099,8 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -1066,7 +1108,8 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -1074,7 +1117,8 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="C76">
         <v>0.5</v>
@@ -1112,7 +1156,8 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>0.1</v>
+        <f>0.1/2</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -1120,7 +1165,8 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>0.1</v>
+        <f t="shared" ref="B81:B89" si="8">0.1/2</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -1128,7 +1174,8 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -1136,7 +1183,8 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -1144,7 +1192,8 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -1152,7 +1201,8 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -1160,7 +1210,8 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -1168,7 +1219,8 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -1176,7 +1228,8 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -1184,7 +1237,8 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>0.1</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
       <c r="C89">
         <v>0.1</v>
@@ -1227,21 +1281,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -1563,8 +1617,8 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <f>1/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f>2/11</f>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -1572,8 +1626,8 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:B46" si="2">1/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" ref="B37:B46" si="2">2/11</f>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -1582,7 +1636,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -1591,7 +1645,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -1600,7 +1654,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -1609,7 +1663,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -1618,7 +1672,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -1627,7 +1681,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -1636,7 +1690,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -1645,7 +1699,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -1654,7 +1708,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="C46">
         <v>0.5</v>
@@ -1684,7 +1738,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
@@ -1692,7 +1746,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
@@ -1700,7 +1754,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -1708,7 +1762,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -1716,7 +1770,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -1724,7 +1778,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
@@ -1732,7 +1786,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -1740,7 +1794,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C56">
         <v>0.4</v>
@@ -1912,8 +1966,8 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <f>1.5/17</f>
-        <v>8.8235294117647065E-2</v>
+        <f>1.6/17</f>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -1921,8 +1975,8 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" ref="B76:B91" si="3">1.5/17</f>
-        <v>8.8235294117647065E-2</v>
+        <f t="shared" ref="B76:B91" si="3">1.6/17</f>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -1931,7 +1985,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -1940,7 +1994,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -1949,7 +2003,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -1958,7 +2012,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -1967,7 +2021,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -1976,7 +2030,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -1985,7 +2039,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -1994,7 +2048,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -2003,7 +2057,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -2012,7 +2066,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -2021,7 +2075,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -2030,7 +2084,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -2039,7 +2093,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
@@ -2048,7 +2102,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -2057,7 +2111,7 @@
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>8.8235294117647065E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
       <c r="C91">
         <v>0.6</v>
@@ -2087,8 +2141,8 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <f>1/13</f>
-        <v>7.6923076923076927E-2</v>
+        <f>1.2/13</f>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
@@ -2096,8 +2150,8 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <f t="shared" ref="B95:B106" si="4">1/13</f>
-        <v>7.6923076923076927E-2</v>
+        <f t="shared" ref="B95:B106" si="4">1.2/13</f>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
@@ -2106,7 +2160,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
@@ -2115,7 +2169,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
@@ -2124,7 +2178,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
@@ -2133,7 +2187,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
@@ -2142,7 +2196,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
@@ -2151,7 +2205,7 @@
       </c>
       <c r="B101">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
@@ -2160,7 +2214,7 @@
       </c>
       <c r="B102">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
@@ -2169,7 +2223,7 @@
       </c>
       <c r="B103">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
@@ -2178,7 +2232,7 @@
       </c>
       <c r="B104">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -2187,7 +2241,7 @@
       </c>
       <c r="B105">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
@@ -2196,7 +2250,7 @@
       </c>
       <c r="B106">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>9.2307692307692299E-2</v>
       </c>
       <c r="C106">
         <v>0.4</v>
@@ -2207,7 +2261,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <f t="shared" ref="B107:B112" si="5">1/6</f>
+        <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -2216,7 +2270,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="B108:B112" si="5">1/6</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -2267,7 +2321,7 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+      <selection activeCell="B100" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2277,13 +2331,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2441,8 +2495,8 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f>1/7</f>
-        <v>0.14285714285714285</v>
+        <f>1.3/7</f>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -2450,8 +2504,8 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B25" si="1">1/7</f>
-        <v>0.14285714285714285</v>
+        <f t="shared" ref="B19:B25" si="1">1.3/7</f>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -2460,7 +2514,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -2469,7 +2523,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -2478,7 +2532,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -2487,7 +2541,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -2496,7 +2550,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <v>0.18571428571428572</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -2505,7 +2559,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <v>0.18571428571428572</v>
       </c>
       <c r="C25">
         <v>0.3</v>
@@ -2516,7 +2570,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
@@ -2524,7 +2578,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C27">
         <v>0.3</v>
@@ -2535,7 +2589,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -2543,7 +2597,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
@@ -2551,7 +2605,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -2559,7 +2613,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -2567,7 +2621,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -2575,7 +2629,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -2583,7 +2637,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -2591,7 +2645,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -2599,7 +2653,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -2607,7 +2661,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="C37">
         <v>0.3</v>
@@ -2618,7 +2672,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -2637,8 +2691,8 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <f>0.8/9</f>
-        <v>8.8888888888888892E-2</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -2646,8 +2700,8 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <f t="shared" ref="B41:B48" si="2">0.8/9</f>
-        <v>8.8888888888888892E-2</v>
+        <f t="shared" ref="B41:B48" si="2">1/9</f>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -2656,7 +2710,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -2665,7 +2719,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -2674,7 +2728,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -2683,7 +2737,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -2692,7 +2746,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -2701,7 +2755,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -2710,7 +2764,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C48">
         <v>0.4</v>
@@ -2751,7 +2805,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -2759,7 +2813,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -2767,7 +2821,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
@@ -2775,7 +2829,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -2783,7 +2837,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
@@ -2791,7 +2845,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -2799,7 +2853,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -2807,7 +2861,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="C59">
         <v>0.4</v>
@@ -2818,7 +2872,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -2826,7 +2880,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="C61">
         <v>0.3</v>
@@ -2837,7 +2891,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -2845,7 +2899,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -2853,7 +2907,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -2861,7 +2915,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -2869,7 +2923,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
@@ -2877,7 +2931,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -2885,7 +2939,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -2893,7 +2947,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -2901,7 +2955,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -2909,7 +2963,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C71">
         <v>0.5</v>
@@ -2920,7 +2974,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -2928,7 +2982,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="C73">
         <v>0.2</v>
@@ -2939,8 +2993,8 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <f>1.5/13</f>
-        <v>0.11538461538461539</v>
+        <f>1.6/13</f>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -2948,8 +3002,8 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B86" si="3">1.5/13</f>
-        <v>0.11538461538461539</v>
+        <f t="shared" ref="B75:B86" si="3">1.6/13</f>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -2958,7 +3012,7 @@
       </c>
       <c r="B76">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -2967,7 +3021,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -2976,7 +3030,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -2985,7 +3039,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -2994,7 +3048,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -3003,7 +3057,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -3012,7 +3066,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -3021,7 +3075,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -3030,7 +3084,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -3039,7 +3093,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -3048,7 +3102,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.12307692307692308</v>
       </c>
       <c r="C86">
         <v>0.5</v>
@@ -3059,7 +3113,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -3067,7 +3121,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -3075,7 +3129,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
@@ -3083,7 +3137,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -3091,7 +3145,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -3099,7 +3153,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -3107,7 +3161,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
@@ -3115,7 +3169,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
@@ -3123,7 +3177,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
@@ -3131,7 +3185,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
@@ -3139,7 +3193,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C97">
         <v>0.3</v>
@@ -3150,7 +3204,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
@@ -3158,7 +3212,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -3172,8 +3226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -3183,13 +3237,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -3402,7 +3456,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
@@ -3410,7 +3464,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
@@ -3418,7 +3472,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
@@ -3426,7 +3480,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -3434,7 +3488,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -3464,8 +3518,8 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <f>1.2/11</f>
-        <v>0.10909090909090909</v>
+        <f>0.8/11</f>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -3473,8 +3527,8 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B41" si="1">1.2/11</f>
-        <v>0.10909090909090909</v>
+        <f t="shared" ref="B33:B42" si="1">0.8/11</f>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -3483,7 +3537,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -3492,7 +3546,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -3501,7 +3555,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -3510,7 +3564,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -3519,7 +3573,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -3528,7 +3582,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -3537,7 +3591,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -3546,7 +3600,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="1"/>
-        <v>0.10909090909090909</v>
+        <v>7.2727272727272738E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -3554,8 +3608,8 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <f>1.2/11</f>
-        <v>0.10909090909090909</v>
+        <f t="shared" si="1"/>
+        <v>7.2727272727272738E-2</v>
       </c>
       <c r="C42">
         <v>0.2</v>
@@ -3566,7 +3620,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -3574,7 +3628,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="C44">
         <v>0.3</v>
@@ -3585,7 +3639,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -3593,7 +3647,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -3601,7 +3655,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -3609,7 +3663,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
@@ -3617,7 +3671,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
@@ -3625,7 +3679,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
@@ -3633,7 +3687,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -3641,7 +3695,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -3649,7 +3703,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -3657,7 +3711,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="C54">
         <v>0.4</v>
@@ -3687,8 +3741,8 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <f>1.5/9</f>
-        <v>0.16666666666666666</v>
+        <f>1.3/9</f>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -3696,8 +3750,8 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <f t="shared" ref="B58:B65" si="2">1.5/9</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" ref="B58:B65" si="2">1.3/9</f>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -3706,7 +3760,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
@@ -3715,7 +3769,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -3724,7 +3778,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
@@ -3733,7 +3787,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -3742,7 +3796,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -3751,7 +3805,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -3760,7 +3814,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.14444444444444446</v>
       </c>
       <c r="C65">
         <v>0.1</v>
@@ -3790,8 +3844,8 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <f>1/7</f>
-        <v>0.14285714285714285</v>
+        <f>0.8/7</f>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -3799,8 +3853,8 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <f t="shared" ref="B69:B74" si="3">1/7</f>
-        <v>0.14285714285714285</v>
+        <f t="shared" ref="B69:B77" si="3">0.8/7</f>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -3809,7 +3863,7 @@
       </c>
       <c r="B70">
         <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -3818,7 +3872,7 @@
       </c>
       <c r="B71">
         <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -3827,7 +3881,7 @@
       </c>
       <c r="B72">
         <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -3836,7 +3890,7 @@
       </c>
       <c r="B73">
         <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -3845,7 +3899,7 @@
       </c>
       <c r="B74">
         <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
+        <v>0.1142857142857143</v>
       </c>
       <c r="C74">
         <v>0.2</v>
@@ -3856,8 +3910,8 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <f>0.4/3</f>
-        <v>0.13333333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -3865,8 +3919,8 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <f>0.4/3</f>
-        <v>0.13333333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -3874,8 +3928,8 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <f>0.4/3</f>
-        <v>0.13333333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.1142857142857143</v>
       </c>
       <c r="C77">
         <v>0.2</v>
@@ -3886,8 +3940,8 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+        <f>0.8/9</f>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -3895,8 +3949,8 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" ref="B79:B86" si="4">1/9</f>
-        <v>0.1111111111111111</v>
+        <f t="shared" ref="B79:B86" si="4">0.8/9</f>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -3905,7 +3959,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -3914,7 +3968,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -3923,7 +3977,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -3932,7 +3986,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -3941,7 +3995,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -3950,7 +4004,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -3959,7 +4013,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="C86">
         <v>0.3</v>
@@ -3970,7 +4024,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -3978,7 +4032,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -3991,21 +4045,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4771,21 +4825,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -5081,8 +5135,8 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <f>1.5/11</f>
-        <v>0.13636363636363635</v>
+        <f>1.8/11</f>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -5090,8 +5144,8 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B42" si="3">1.5/11</f>
-        <v>0.13636363636363635</v>
+        <f t="shared" ref="B33:B42" si="3">1.8/11</f>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -5100,7 +5154,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -5109,7 +5163,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -5118,7 +5172,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -5127,7 +5181,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -5136,7 +5190,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -5145,7 +5199,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -5154,7 +5208,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -5163,7 +5217,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -5172,7 +5226,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <v>0.16363636363636364</v>
       </c>
       <c r="C42">
         <v>0.2</v>
@@ -5183,7 +5237,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -5191,7 +5245,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -5199,7 +5253,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C45">
         <v>0.3</v>
@@ -5210,8 +5264,8 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <f>1.5/9</f>
-        <v>0.16666666666666666</v>
+        <f>1.6/9</f>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -5219,8 +5273,8 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <f t="shared" ref="B47:B54" si="4">1.5/9</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" ref="B47:B54" si="4">1.6/9</f>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -5229,7 +5283,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
@@ -5238,7 +5292,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
@@ -5247,7 +5301,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
@@ -5256,7 +5310,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -5265,7 +5319,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -5274,7 +5328,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -5283,7 +5337,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="C54">
         <v>0.2</v>
@@ -5313,8 +5367,8 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <f>1/10</f>
-        <v>0.1</v>
+        <f>1.2/10</f>
+        <v>0.12</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -5322,8 +5376,8 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <f t="shared" ref="B58:B66" si="5">1/10</f>
-        <v>0.1</v>
+        <f t="shared" ref="B58:B66" si="5">1.2/10</f>
+        <v>0.12</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -5332,7 +5386,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
@@ -5341,7 +5395,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -5350,7 +5404,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
@@ -5359,7 +5413,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -5368,7 +5422,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -5377,7 +5431,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -5386,7 +5440,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -5395,7 +5449,7 @@
       </c>
       <c r="B66">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="C66">
         <v>0.3</v>
@@ -5425,8 +5479,8 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <f>1.5/8</f>
-        <v>0.1875</v>
+        <f>1.7/8</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -5434,8 +5488,8 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" ref="B70:B76" si="6">1.5/8</f>
-        <v>0.1875</v>
+        <f t="shared" ref="B70:B76" si="6">1.7/8</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -5444,7 +5498,7 @@
       </c>
       <c r="B71">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -5453,7 +5507,7 @@
       </c>
       <c r="B72">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -5462,7 +5516,7 @@
       </c>
       <c r="B73">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -5471,7 +5525,7 @@
       </c>
       <c r="B74">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -5480,7 +5534,7 @@
       </c>
       <c r="B75">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -5489,7 +5543,7 @@
       </c>
       <c r="B76">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0.21249999999999999</v>
       </c>
       <c r="C76">
         <v>0.2</v>
@@ -5500,7 +5554,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -5508,7 +5562,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="C78">
         <v>0.2</v>
@@ -5519,8 +5573,8 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <f>1/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f>1.2/11</f>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -5528,8 +5582,8 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" ref="B80:B89" si="7">1/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" ref="B80:B89" si="7">1.2/11</f>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -5538,7 +5592,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -5547,7 +5601,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -5556,7 +5610,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -5565,7 +5619,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -5574,7 +5628,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -5583,7 +5637,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -5592,7 +5646,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -5601,7 +5655,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -5610,7 +5664,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="7"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.10909090909090909</v>
       </c>
       <c r="C89">
         <v>0.4</v>
@@ -5621,7 +5675,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -5629,7 +5683,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -6561,7 +6615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
@@ -7397,7 +7451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
@@ -7610,7 +7664,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B30" si="2">1/9</f>
+        <f t="shared" ref="B22:B29" si="2">1/9</f>
         <v>0.1111111111111111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix lyrics index reader bug
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/LyricsData.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/LyricsData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="0" windowWidth="16680" windowHeight="12645" tabRatio="611" activeTab="7"/>
+    <workbookView xWindow="12120" yWindow="0" windowWidth="16680" windowHeight="12645" tabRatio="611" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="tokiwa1" sheetId="1" r:id="rId1"/>
@@ -5696,8 +5696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -5754,8 +5754,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>8.3333000000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -5814,8 +5813,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:B17" si="1">1/7</f>
-        <v>0.14285714285714285</v>
+        <v>0.14285700000000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -5823,7 +5821,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B13:B17" si="1">1/7</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -6615,8 +6613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -6655,7 +6653,6 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>

</xml_diff>